<commit_message>
CC identifiers version 2312
Update Current Channel identifiers for version 2312 (Build 17126.20132)
</commit_message>
<xml_diff>
--- a/Microsoft 365/Current Channel/outlookmmseditcontrols.xlsx
+++ b/Microsoft 365/Current Channel/outlookmmseditcontrols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RibbonXThing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TcidDocs\CCNov2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C3F991D-8BC3-4430-8252-CA9DD9BF9402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F2A5D8-2381-41BC-ADA9-C6CE22F5A1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15345"/>
+    <workbookView xWindow="0" yWindow="5415" windowWidth="51600" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="outlookmmseditcontrols" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,19 +649,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -672,19 +672,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.7999816888943144"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -695,19 +695,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.5999938962981048"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -718,19 +718,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -741,19 +741,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -764,19 +764,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -812,7 +812,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1342,20 +1342,20 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.875" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="1" max="1" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.625" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>25419</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>16164</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>13289</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>12597</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>13343</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>13312</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>13315</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>13313</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>13318</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>13318</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>14349</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>13293</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>13316</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>20868</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>13303</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>13317</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>13319</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>2707</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>13294</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>13308</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>13309</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>22110</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>22111</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>19623</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>19624</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>19625</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>22112</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>22113</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>22338</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>11323</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>2521</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="B54" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>19211</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="B55" t="s">
         <v>9</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>19212</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="B56" t="s">
         <v>9</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>19214</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="B57" t="s">
         <v>9</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>19213</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="B58" t="s">
         <v>9</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>19215</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>9340</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>5933</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>7714</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>16164</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>32712</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>24438</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>22143</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>7391</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>25419</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>22377</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>5598</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>20108</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>26904</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>27010</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>27007</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>27006</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>27085</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>27142</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>27805</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>27877</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>27</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>27964</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="B90" t="s">
         <v>9</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>33991</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>18148</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>25295</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>34474</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="B94" t="s">
         <v>24</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>33917</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>33912</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>20423</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>20424</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>20425</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>20426</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>20440</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>20441</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>32646</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>20442</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>20443</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>20444</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>20445</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>18792</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8">
       <c r="B108" t="s">
         <v>9</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>33940</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8">
       <c r="B109" t="s">
         <v>9</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>33939</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>61</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>62</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>18244</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>19139</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>19140</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>20802</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>24423</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>33755</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>33756</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>24850</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>25368</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>24207</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>24952</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>24424</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="B127" t="s">
         <v>9</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>24421</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>22547</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>125</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>20511</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>34138</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>127</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>34139</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>128</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>27331</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>27363</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>27364</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>131</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>27365</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>132</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>27366</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>133</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>18158</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>134</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>26945</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>135</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>27265</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>136</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>27266</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>137</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>27267</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>138</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>27545</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>139</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>33737</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="B144" t="s">
         <v>9</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>33739</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>33738</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="B146" t="s">
         <v>9</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>33740</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>141</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>27005</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>85</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>27007</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>142</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>27021</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>86</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>27006</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>143</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>27058</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>144</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>27302</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>60</v>
       </c>

</xml_diff>